<commit_message>
Added my name to group contribution
</commit_message>
<xml_diff>
--- a/Group Contribution/MXB226GroupProjectContributions2019.xlsx
+++ b/Group Contribution/MXB226GroupProjectContributions2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\MXB226\Modelling-an-Electronic-Component-Case-Study\Group Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E52CB7-C87D-4ECA-A86C-B2D70147654B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48D9177-EBC8-4988-8647-211C1D05C668}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>Packed storage</t>
   </si>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +925,9 @@
       <c r="B12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
@@ -989,7 +991,9 @@
       <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
@@ -1005,7 +1009,9 @@
       <c r="B22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
@@ -1101,7 +1107,9 @@
       <c r="B34" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
@@ -1229,7 +1237,9 @@
       <c r="B50" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>

</xml_diff>

<commit_message>
Group Contribution so far
</commit_message>
<xml_diff>
--- a/Group Contribution/MXB226GroupProjectContributions2019.xlsx
+++ b/Group Contribution/MXB226GroupProjectContributions2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\MXB226\Modelling-an-Electronic-Component-Case-Study\Group Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48D9177-EBC8-4988-8647-211C1D05C668}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2E6075-2E8F-443F-85FE-FF4BD77D96D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>Packed storage</t>
   </si>
@@ -198,10 +198,10 @@
     <t>Jean-Luc</t>
   </si>
   <si>
-    <t>Azure, Faris, Jean-luc</t>
-  </si>
-  <si>
     <t>Azure</t>
+  </si>
+  <si>
+    <t>Faris</t>
   </si>
 </sst>
 </file>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +818,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -908,7 +908,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -959,7 +959,9 @@
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
@@ -975,7 +977,9 @@
       <c r="B18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
@@ -1043,7 +1047,9 @@
       <c r="B26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
@@ -1059,7 +1065,9 @@
       <c r="B28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
@@ -1075,7 +1083,9 @@
       <c r="B30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>

</xml_diff>

<commit_message>
Group contribution and report
</commit_message>
<xml_diff>
--- a/Group Contribution/MXB226GroupProjectContributions2019.xlsx
+++ b/Group Contribution/MXB226GroupProjectContributions2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\MXB226\Modelling-an-Electronic-Component-Case-Study\Group Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2E6075-2E8F-443F-85FE-FF4BD77D96D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75F8C38-E9FE-4740-BABF-68D168115AE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Packed storage</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Faris</t>
+  </si>
+  <si>
+    <t>Azure/Jean-Luc</t>
   </si>
 </sst>
 </file>
@@ -784,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +839,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1151,7 +1154,9 @@
       <c r="B38" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
@@ -1167,7 +1172,9 @@
       <c r="B40" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
@@ -1183,7 +1190,9 @@
       <c r="B42" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
@@ -1199,7 +1208,9 @@
       <c r="B44" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>

</xml_diff>

<commit_message>
Report and code updates
</commit_message>
<xml_diff>
--- a/Group Contribution/MXB226GroupProjectContributions2019.xlsx
+++ b/Group Contribution/MXB226GroupProjectContributions2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\MXB226\Modelling-an-Electronic-Component-Case-Study\Group Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75F8C38-E9FE-4740-BABF-68D168115AE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0587DE-0061-41A6-88F4-FFFDB0BEBB30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -788,7 +788,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>